<commit_message>
Confirm replication & fix [weightab] bug
</commit_message>
<xml_diff>
--- a/Outputs/manuscript/t2-caseload.xlsx
+++ b/Outputs/manuscript/t2-caseload.xlsx
@@ -2575,7 +2575,7 @@
         <v>22.542368594070389</v>
       </c>
       <c r="D2" s="72">
-        <v>22.845221309041861</v>
+        <v>22.84522130904185</v>
       </c>
     </row>
     <row r="3">
@@ -2603,7 +2603,7 @@
         <v>10.192316614668631</v>
       </c>
       <c r="D4" s="78">
-        <v>8.1513283337240523</v>
+        <v>8.1513283337240612</v>
       </c>
     </row>
     <row r="5">
@@ -2667,10 +2667,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="91">
-        <v>1.425994131584104</v>
+        <v>1.425994131584102</v>
       </c>
       <c r="C9" s="92">
-        <v>1.392317343267196</v>
+        <v>1.392317343267194</v>
       </c>
       <c r="D9" s="93">
         <v>1.426858732406254</v>
@@ -2684,10 +2684,10 @@
         <v>-1.0876933510429161</v>
       </c>
       <c r="C10" s="95">
-        <v>-1.168611009283498</v>
+        <v>-1.1686110092834989</v>
       </c>
       <c r="D10" s="96">
-        <v>-0.97854815528162531</v>
+        <v>-0.97854815528160588</v>
       </c>
     </row>
     <row r="11">
@@ -2695,10 +2695,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="97">
-        <v>2.9786569508930829</v>
+        <v>2.9786569508931442</v>
       </c>
       <c r="C11" s="98">
-        <v>3.123659623698209</v>
+        <v>3.1236596236982099</v>
       </c>
       <c r="D11" s="99">
         <v>3.3155023501835901</v>
@@ -2715,7 +2715,7 @@
         <v>1.3205404370178739</v>
       </c>
       <c r="D12" s="102">
-        <v>1.358856305377133</v>
+        <v>1.3588563053771521</v>
       </c>
     </row>
     <row r="13">
@@ -2723,10 +2723,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="103">
-        <v>2.9852350131828209</v>
+        <v>2.98523501318282</v>
       </c>
       <c r="C13" s="104">
-        <v>3.1328819952056932</v>
+        <v>3.132881995205492</v>
       </c>
       <c r="D13" s="105">
         <v>3.316215397915002</v>
@@ -2743,7 +2743,7 @@
         <v>2.518934921575696</v>
       </c>
       <c r="D14" s="108">
-        <v>2.8060647054831831</v>
+        <v>2.8060647054832022</v>
       </c>
     </row>
     <row r="15">
@@ -2751,13 +2751,13 @@
         <v>1</v>
       </c>
       <c r="B15" s="109">
-        <v>3.0121825195860561</v>
+        <v>3.0121825195860241</v>
       </c>
       <c r="C15" s="110">
-        <v>3.1622207095881358</v>
+        <v>3.1622207095882948</v>
       </c>
       <c r="D15" s="111">
-        <v>3.3448661582872261</v>
+        <v>3.344866158287227</v>
       </c>
     </row>
     <row r="16">
@@ -2779,10 +2779,10 @@
         <v>1</v>
       </c>
       <c r="B17" s="115">
-        <v>0.48172438365227949</v>
+        <v>0.48172438365227971</v>
       </c>
       <c r="C17" s="116">
-        <v>0.48827174673092288</v>
+        <v>0.488271746730923</v>
       </c>
       <c r="D17" s="117">
         <v>0.50541704621996753</v>
@@ -2793,13 +2793,13 @@
         <v>9</v>
       </c>
       <c r="B18" s="118">
-        <v>0.94477636554091027</v>
+        <v>0.94477636554091038</v>
       </c>
       <c r="C18" s="119">
-        <v>0.91024029646014204</v>
+        <v>0.91024029646014215</v>
       </c>
       <c r="D18" s="120">
-        <v>0.65171488956250678</v>
+        <v>0.65171488956250656</v>
       </c>
     </row>
     <row r="19">
@@ -2807,10 +2807,10 @@
         <v>1</v>
       </c>
       <c r="B19" s="121">
-        <v>0.650622214752127</v>
+        <v>0.65062221475212678</v>
       </c>
       <c r="C19" s="122">
-        <v>0.64149908945368384</v>
+        <v>0.64149908945368361</v>
       </c>
       <c r="D19" s="123">
         <v>0.63462036668167532</v>
@@ -2821,13 +2821,13 @@
         <v>10</v>
       </c>
       <c r="B20" s="124">
-        <v>-0.99314719384658889</v>
+        <v>-0.99314719384658878</v>
       </c>
       <c r="C20" s="125">
         <v>-0.84521752848743936</v>
       </c>
       <c r="D20" s="126">
-        <v>-1.2148272520982519</v>
+        <v>-1.214827252098253</v>
       </c>
     </row>
     <row r="21">
@@ -2857,7 +2857,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="131">
-        <v>0.90974262819674889</v>
+        <v>0.90974262819674878</v>
       </c>
     </row>
     <row r="24">
@@ -2873,7 +2873,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="133">
-        <v>0.018081189215723801</v>
+        <v>0.0180811892157237</v>
       </c>
     </row>
     <row r="26">
@@ -2887,7 +2887,7 @@
         <v>-0.13227455398286381</v>
       </c>
       <c r="D26" s="136">
-        <v>3.3658663158880362</v>
+        <v>3.3658663158880171</v>
       </c>
     </row>
     <row r="27">
@@ -2895,13 +2895,13 @@
         <v>1</v>
       </c>
       <c r="B27" s="137">
-        <v>3.2625453487762428</v>
+        <v>3.26254534877638</v>
       </c>
       <c r="C27" s="138">
-        <v>3.6544560342196171</v>
+        <v>3.6544560342194812</v>
       </c>
       <c r="D27" s="139">
-        <v>3.5659531407365481</v>
+        <v>3.565953140736549</v>
       </c>
     </row>
     <row r="28">

</xml_diff>

<commit_message>
Resubmission version with data
</commit_message>
<xml_diff>
--- a/Outputs/manuscript/t2-caseload.xlsx
+++ b/Outputs/manuscript/t2-caseload.xlsx
@@ -86,459 +86,447 @@
     <numFmt numFmtId="169" formatCode="#0.00\*_*_*"/>
     <numFmt numFmtId="170" formatCode="#0.00\*\*_*"/>
   </numFmts>
-  <fonts count="184">
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <b/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
+  <fonts count="181">
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <b/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <b/>
     </font>
     <font>
       <sz val="11"/>
@@ -865,7 +853,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="152">
+  <borders count="149">
     <border>
       <left/>
       <right/>
@@ -1892,13 +1880,6 @@
       <left style="none"/>
       <right style="none"/>
       <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
       <bottom style="thin"/>
       <diagonal style="none"/>
     </border>
@@ -1906,21 +1887,7 @@
       <left style="none"/>
       <right style="none"/>
       <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
       <bottom style="thin"/>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
       <diagonal style="none"/>
     </border>
     <border>
@@ -1934,7 +1901,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -2516,27 +2483,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="178" fillId="0" borderId="146" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="179" fillId="0" borderId="147" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="180" fillId="0" borderId="148" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="181" fillId="0" borderId="149" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="182" fillId="0" borderId="150" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="183" fillId="0" borderId="151" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="178" fillId="0" borderId="146" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="179" fillId="0" borderId="147" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="180" fillId="0" borderId="148" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2572,10 +2527,10 @@
         <v>22.514249648796291</v>
       </c>
       <c r="C2" s="71">
-        <v>22.5423685940704</v>
+        <v>22.542368594070389</v>
       </c>
       <c r="D2" s="72">
-        <v>22.84522130904185</v>
+        <v>22.845221309041861</v>
       </c>
     </row>
     <row r="3">
@@ -2586,7 +2541,7 @@
         <v>5.05099567294587</v>
       </c>
       <c r="C3" s="74">
-        <v>4.9914988197683492</v>
+        <v>4.9914988197683501</v>
       </c>
       <c r="D3" s="75">
         <v>4.9010901894850134</v>
@@ -2603,7 +2558,7 @@
         <v>10.192316614668631</v>
       </c>
       <c r="D4" s="78">
-        <v>8.1513283337240612</v>
+        <v>8.1513283337240523</v>
       </c>
     </row>
     <row r="5">
@@ -2611,10 +2566,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="79">
-        <v>2.9558869297900738</v>
+        <v>2.9558869297900752</v>
       </c>
       <c r="C5" s="80">
-        <v>3.0211278568390938</v>
+        <v>3.0211278568390929</v>
       </c>
       <c r="D5" s="81">
         <v>2.860444175899044</v>
@@ -2653,7 +2608,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="88">
-        <v>0.97533653023810185</v>
+        <v>0.97533653023810207</v>
       </c>
       <c r="C8" s="89">
         <v>2.5167769474490251</v>
@@ -2681,13 +2636,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="94">
-        <v>-1.087693351042915</v>
+        <v>-1.087693351042927</v>
       </c>
       <c r="C10" s="95">
-        <v>-1.168611009283502</v>
+        <v>-1.1686110092835129</v>
       </c>
       <c r="D10" s="96">
-        <v>-0.97854815528160644</v>
+        <v>-0.97854815528164496</v>
       </c>
     </row>
     <row r="11">
@@ -2695,13 +2650,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="97">
-        <v>2.9786569508933298</v>
+        <v>2.9786569508931442</v>
       </c>
       <c r="C11" s="98">
-        <v>3.1236596236984431</v>
+        <v>3.1236596236980931</v>
       </c>
       <c r="D11" s="99">
-        <v>3.315502350183924</v>
+        <v>3.3155023501835612</v>
       </c>
     </row>
     <row r="12">
@@ -2709,13 +2664,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="100">
-        <v>1.383838220948105</v>
+        <v>1.3838382209480931</v>
       </c>
       <c r="C12" s="101">
-        <v>1.320540437017871</v>
+        <v>1.3205404370178599</v>
       </c>
       <c r="D12" s="102">
-        <v>1.3588563053771521</v>
+        <v>1.3588563053771141</v>
       </c>
     </row>
     <row r="13">
@@ -2723,13 +2678,13 @@
         <v>1</v>
       </c>
       <c r="B13" s="103">
-        <v>2.9852350131830661</v>
+        <v>2.9852350131827898</v>
       </c>
       <c r="C13" s="104">
-        <v>3.132881995205536</v>
+        <v>3.132881995205941</v>
       </c>
       <c r="D13" s="105">
-        <v>3.3162153979152218</v>
+        <v>3.3162153979151392</v>
       </c>
     </row>
     <row r="14">
@@ -2737,13 +2692,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="106">
-        <v>2.383678114771969</v>
+        <v>2.3836781147719579</v>
       </c>
       <c r="C14" s="107">
-        <v>2.5189349215756929</v>
+        <v>2.5189349215756822</v>
       </c>
       <c r="D14" s="108">
-        <v>2.8060647054832009</v>
+        <v>2.806064705483164</v>
       </c>
     </row>
     <row r="15">
@@ -2751,13 +2706,13 @@
         <v>1</v>
       </c>
       <c r="B15" s="109">
-        <v>3.012182519586541</v>
+        <v>3.0121825195861738</v>
       </c>
       <c r="C15" s="110">
-        <v>3.1622207095880781</v>
+        <v>3.1622207095883832</v>
       </c>
       <c r="D15" s="111">
-        <v>3.3448661582873922</v>
+        <v>3.344866158287199</v>
       </c>
     </row>
     <row r="16">
@@ -2782,10 +2737,10 @@
         <v>0.48172438365227988</v>
       </c>
       <c r="C17" s="116">
-        <v>0.48827174673092288</v>
+        <v>0.488271746730923</v>
       </c>
       <c r="D17" s="117">
-        <v>0.50541704621996764</v>
+        <v>0.50541704621996697</v>
       </c>
     </row>
     <row r="18">
@@ -2793,13 +2748,13 @@
         <v>9</v>
       </c>
       <c r="B18" s="118">
-        <v>0.94477636554091038</v>
+        <v>0.94477636554091027</v>
       </c>
       <c r="C18" s="119">
         <v>0.91024029646014204</v>
       </c>
       <c r="D18" s="120">
-        <v>0.65171488956250645</v>
+        <v>0.65171488956250656</v>
       </c>
     </row>
     <row r="19">
@@ -2810,10 +2765,10 @@
         <v>0.65062221475212689</v>
       </c>
       <c r="C19" s="122">
-        <v>0.64149908945368361</v>
+        <v>0.6414990894536835</v>
       </c>
       <c r="D19" s="123">
-        <v>0.63462036668167532</v>
+        <v>0.63462036668167543</v>
       </c>
     </row>
     <row r="20">
@@ -2821,13 +2776,13 @@
         <v>10</v>
       </c>
       <c r="B20" s="124">
-        <v>-0.99314719384658889</v>
+        <v>-0.99314719384658878</v>
       </c>
       <c r="C20" s="125">
-        <v>-0.84521752848743936</v>
+        <v>-0.84521752848743925</v>
       </c>
       <c r="D20" s="126">
-        <v>-1.214827252098253</v>
+        <v>-1.2148272520982519</v>
       </c>
     </row>
     <row r="21">
@@ -2841,7 +2796,7 @@
         <v>1.1567206395463649</v>
       </c>
       <c r="D21" s="129">
-        <v>1.1640110475802481</v>
+        <v>1.164011047580247</v>
       </c>
     </row>
     <row r="22">
@@ -2857,7 +2812,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="131">
-        <v>0.90974262819675034</v>
+        <v>0.90974262819674945</v>
       </c>
     </row>
     <row r="24">
@@ -2873,7 +2828,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="133">
-        <v>0.0180811892157237</v>
+        <v>0.018081189215723801</v>
       </c>
     </row>
     <row r="26">
@@ -2881,13 +2836,13 @@
         <v>13</v>
       </c>
       <c r="B26" s="134">
-        <v>3.3912368556378052</v>
+        <v>3.3912368556378159</v>
       </c>
       <c r="C26" s="135">
-        <v>-0.13227455398286031</v>
+        <v>-0.1322745539828496</v>
       </c>
       <c r="D26" s="136">
-        <v>3.3658663158880171</v>
+        <v>3.365866315888054</v>
       </c>
     </row>
     <row r="27">
@@ -2895,13 +2850,13 @@
         <v>1</v>
       </c>
       <c r="B27" s="137">
-        <v>3.2625453487763818</v>
+        <v>3.2625453487766229</v>
       </c>
       <c r="C27" s="138">
-        <v>3.654456034219514</v>
+        <v>3.654456034219733</v>
       </c>
       <c r="D27" s="139">
-        <v>3.5659531407361991</v>
+        <v>3.5659531407363541</v>
       </c>
     </row>
     <row r="28">
@@ -2936,15 +2891,9 @@
       <c r="A30" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="147">
-        <v>17.90128200436645</v>
-      </c>
-      <c r="C30" s="149">
-        <v>17.90128200436645</v>
-      </c>
-      <c r="D30" s="151">
-        <v>17.90128200436645</v>
-      </c>
+      <c r="B30" s="146"/>
+      <c r="C30" s="147"/>
+      <c r="D30" s="148"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>